<commit_message>
Added Place_Rn to Export Buhgalteria
</commit_message>
<xml_diff>
--- a/XML/removed_from_TO.xlsx
+++ b/XML/removed_from_TO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t>Контрагент</t>
   </si>
@@ -38,139 +38,166 @@
     <t>Дата снятия с ТО</t>
   </si>
   <si>
-    <t>УП "Вода 2000"</t>
-  </si>
-  <si>
-    <t>УП "Либра-2000"</t>
-  </si>
-  <si>
-    <t>ИП Балабуха Сергей Александрович</t>
-  </si>
-  <si>
-    <t>ООО "Автопривоз"</t>
-  </si>
-  <si>
-    <t>ЗАО "Ассистанс Хэлс"</t>
-  </si>
-  <si>
-    <t>ОДО "Дизайн окна"</t>
-  </si>
-  <si>
-    <t>ООО "Трансмайл"</t>
-  </si>
-  <si>
-    <t>ЧП "Тропикана Трэвел"</t>
-  </si>
-  <si>
-    <t>ООО "Автопривоз Трэйдинг"</t>
-  </si>
-  <si>
-    <t>ЧП "Скарпетта С"</t>
-  </si>
-  <si>
-    <t>Частное предприятие "АвилонАвто"</t>
-  </si>
-  <si>
-    <t>ИП Чистякова Татьяна Иосифовна</t>
-  </si>
-  <si>
-    <t>Частное предприятие "ПОЛАДИЗ"</t>
-  </si>
-  <si>
-    <t>ООО "ЮКА-стайл"</t>
-  </si>
-  <si>
-    <t>ООО "ЗаймКапитал"</t>
-  </si>
-  <si>
-    <t>ИП Максимович Юлия Геннадьевна</t>
-  </si>
-  <si>
-    <t>ИП Малинин Александр Владимирович</t>
-  </si>
-  <si>
-    <t>Частное предприятие  "БЕЛ ТОРГ ГРУПП"</t>
-  </si>
-  <si>
-    <t>ИП Волчек Анатолий Васильевич</t>
-  </si>
-  <si>
-    <t>ИП Сеникович Светлана Валентиновна</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ООО "СветлПроДа"</t>
-  </si>
-  <si>
-    <t>ИП Светогор Валентина Васильевна</t>
-  </si>
-  <si>
-    <t>ИП Мехдиев Узеир Мехдипаша Оглы</t>
-  </si>
-  <si>
-    <t>ОДО "Экспресслинии"</t>
-  </si>
-  <si>
-    <t>ООО БЕЛКРЕП</t>
-  </si>
-  <si>
-    <t>ООО Бабочки</t>
-  </si>
-  <si>
-    <t>ИП Дементьев Владимир Владимирович</t>
-  </si>
-  <si>
-    <t>000 "Коммерческий курьер"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Бобруйский ф-л Автобусный парк № 2 ОАО "Могилевоблавтотранс"</t>
-  </si>
-  <si>
-    <t>ИП Карпов Виталий Исаевич</t>
-  </si>
-  <si>
-    <t>ООО "Крагор"</t>
-  </si>
-  <si>
-    <t>ОДО Лемиан</t>
-  </si>
-  <si>
-    <t>Частное предприятие "БарАлекс Транс"</t>
-  </si>
-  <si>
-    <t>ИП Бусель Татьяна Ивановна</t>
-  </si>
-  <si>
-    <t>OOO "АрсСтройНова"</t>
-  </si>
-  <si>
-    <t>"Частное предприятие" "Русакович В.Н."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ИП Во Нам Лыонг  </t>
-  </si>
-  <si>
-    <t>ИП Зененкова Виктория Олеговна</t>
-  </si>
-  <si>
-    <t>ИП Виденькина Марина Владимировна</t>
-  </si>
-  <si>
-    <t>ИП Стельмак Ирины Павловна</t>
-  </si>
-  <si>
-    <t>Частное предприятие "Викас-глобал"</t>
-  </si>
-  <si>
-    <t>ИП Зеленцов Олег Витальевич</t>
-  </si>
-  <si>
-    <t>ИП Коваленко Андрей Николаевич</t>
-  </si>
-  <si>
-    <t>ИП Скучко Сергей Васильевич</t>
-  </si>
-  <si>
-    <t>ИП Платонов Дмитрий Анатольевич</t>
+    <t>Учреждение "Минское городское управление Министерства по чрезвычайным ситуациям Республики Беларусь"</t>
+  </si>
+  <si>
+    <t>УП "18"</t>
+  </si>
+  <si>
+    <t>ОДО "Старый стиль"</t>
+  </si>
+  <si>
+    <t>ИП Лучко Нелли Николаевна</t>
+  </si>
+  <si>
+    <t>УП "Звезда Удачи"</t>
+  </si>
+  <si>
+    <t>ООО "Никулич и Ко"</t>
+  </si>
+  <si>
+    <t>ЧУП "Бурая Ю.В."</t>
+  </si>
+  <si>
+    <t>ООО "Автотехцентр Варди"</t>
+  </si>
+  <si>
+    <t>ИП Альховик Александр Михайлович</t>
+  </si>
+  <si>
+    <t>ООО "Минэкспресс"</t>
+  </si>
+  <si>
+    <t>СООО "Аргомунт-центр"</t>
+  </si>
+  <si>
+    <t>ЧП "Аланавто"</t>
+  </si>
+  <si>
+    <t>Частное предприятие  " Филл-В"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> МКСК"Минск-арена"</t>
+  </si>
+  <si>
+    <t>ИП Тригубова Светлана Александровна</t>
+  </si>
+  <si>
+    <t>ООО "Сетелайт"</t>
+  </si>
+  <si>
+    <t>Строительное унитарное предприятие "Алютерм" ОАО "Минскпромстрой"</t>
+  </si>
+  <si>
+    <t>ЧТУП "АвтоШтарк"</t>
+  </si>
+  <si>
+    <t>ООО "Курсор- Голд"</t>
+  </si>
+  <si>
+    <t>ИП Демух Татьяна Геннадьевна</t>
+  </si>
+  <si>
+    <t>ООО "ЧемоданМаркет"</t>
+  </si>
+  <si>
+    <t>ИП Вязовская Кристина Георгиевна</t>
+  </si>
+  <si>
+    <t>Частное предприятие  "ТурбоСтупа"</t>
+  </si>
+  <si>
+    <t>ИП Демицкая Виктория Михайловна</t>
+  </si>
+  <si>
+    <t>ООО "Этако"</t>
+  </si>
+  <si>
+    <t>ЧП "Белтрэйдмастер"</t>
+  </si>
+  <si>
+    <t>ООО "Альтерра-Транс"</t>
+  </si>
+  <si>
+    <t>Частное предприятие "РеалТеплоСервис"</t>
+  </si>
+  <si>
+    <t>Частное предприятие "Токантинс"</t>
+  </si>
+  <si>
+    <t>ООО "БонаПай"</t>
+  </si>
+  <si>
+    <t>ООО "Лесок Эксперт"</t>
+  </si>
+  <si>
+    <t>ИП Бригадир Вера Сергеевна</t>
+  </si>
+  <si>
+    <t>ИП Казеко Валентина Ивановна</t>
+  </si>
+  <si>
+    <t>ИП Ляцкий Дмитрий Николаевич</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Могилевский ф-л Автобусный парк " № 1 ОАО "Могилевоблавтотранс"</t>
+  </si>
+  <si>
+    <t>ИП Сафронова Нина Ивановна</t>
+  </si>
+  <si>
+    <t>ИП Бабухина Алла Викторовна</t>
+  </si>
+  <si>
+    <t>ИП Скрипунов Михаил Андреевич</t>
+  </si>
+  <si>
+    <t>ИП Дзыгун Татьяна Иосифовна</t>
+  </si>
+  <si>
+    <t>ИП Шестеркина Елена Станиславовна</t>
+  </si>
+  <si>
+    <t>ИП Горбачев Владимир Иванович</t>
+  </si>
+  <si>
+    <t>ИП Дайнеко Виктория Ивановна</t>
+  </si>
+  <si>
+    <t>ООО "Содружество-Авто"</t>
+  </si>
+  <si>
+    <t>"Частное предприятие" "Прохоров"</t>
+  </si>
+  <si>
+    <t>"Частное предприятие" "Сирик С.П."</t>
+  </si>
+  <si>
+    <t>ЧУП по оказанию услуг "Садко-авто"</t>
+  </si>
+  <si>
+    <t>ОДО АвтоТрансЛайн</t>
+  </si>
+  <si>
+    <t>ИП Гуринович Наталья Викторовна</t>
+  </si>
+  <si>
+    <t>ИП Лошанков  Сергей Михайлович</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Частное ломбардное унитарное предприятие "ИГЛЕНАГРУПП"</t>
+  </si>
+  <si>
+    <t>ИП Белуга Сергей Петрович</t>
+  </si>
+  <si>
+    <t>ИП Кожевников Владимир Алексеевич</t>
+  </si>
+  <si>
+    <t>ИП Каковко Сергей Васильевич</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ИП Зыонг Ань Туан  </t>
   </si>
 </sst>
 </file>
@@ -500,7 +527,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -529,13 +556,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>101458075</v>
+        <v>100124836</v>
       </c>
       <c r="C2">
-        <v>21004472</v>
+        <v>20717247</v>
       </c>
       <c r="D2" s="2">
-        <v>43070.418749999997</v>
+        <v>43104.500694444447</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -543,13 +570,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>190221473</v>
+        <v>100177173</v>
       </c>
       <c r="C3">
-        <v>20616237</v>
+        <v>21002405</v>
       </c>
       <c r="D3" s="2">
-        <v>43073.430555555555</v>
+        <v>43105.465277777781</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -557,13 +584,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>190238191</v>
+        <v>190050193</v>
       </c>
       <c r="C4">
-        <v>21000648</v>
+        <v>20614259</v>
       </c>
       <c r="D4" s="2">
-        <v>43074.619444444441</v>
+        <v>43122.489583333336</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -571,13 +598,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>190436756</v>
+        <v>190252263</v>
       </c>
       <c r="C5">
-        <v>21003798</v>
+        <v>21002326</v>
       </c>
       <c r="D5" s="2">
-        <v>43096.431250000001</v>
+        <v>43105.474999999999</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -585,13 +612,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>190512752</v>
+        <v>190414788</v>
       </c>
       <c r="C6">
-        <v>21001394</v>
+        <v>21400235</v>
       </c>
       <c r="D6" s="2">
-        <v>43088.725694444445</v>
+        <v>43111.736805555556</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -599,13 +626,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>190593102</v>
+        <v>190559938</v>
       </c>
       <c r="C7">
-        <v>20700900</v>
+        <v>21001189</v>
       </c>
       <c r="D7" s="2">
-        <v>43089.477777777778</v>
+        <v>43115.394444444442</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -613,139 +640,139 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>190593102</v>
+        <v>190559938</v>
       </c>
       <c r="C8">
-        <v>20701205</v>
+        <v>21100056</v>
       </c>
       <c r="D8" s="2">
-        <v>43089.477083333331</v>
+        <v>43115.396527777775</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>190593102</v>
+        <v>190590795</v>
       </c>
       <c r="C9">
-        <v>21004244</v>
+        <v>21003934</v>
       </c>
       <c r="D9" s="2">
-        <v>43089.479166666664</v>
+        <v>43123.551388888889</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>190615425</v>
+        <v>190657573</v>
       </c>
       <c r="C10">
-        <v>21003353</v>
+        <v>20616512</v>
       </c>
       <c r="D10" s="2">
-        <v>43073.543749999997</v>
+        <v>43103.523611111108</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>190615425</v>
+        <v>190747684</v>
       </c>
       <c r="C11">
-        <v>21400470</v>
+        <v>21000248</v>
       </c>
       <c r="D11" s="2">
-        <v>43073.543055555558</v>
+        <v>43104.553472222222</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>190819980</v>
+        <v>190764408</v>
       </c>
       <c r="C12">
-        <v>20616557</v>
+        <v>21003011</v>
       </c>
       <c r="D12" s="2">
-        <v>43080.536805555559</v>
+        <v>43103.579861111109</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>190978197</v>
+        <v>190810279</v>
       </c>
       <c r="C13">
-        <v>21100204</v>
+        <v>20717244</v>
       </c>
       <c r="D13" s="2">
-        <v>43075.429166666669</v>
+        <v>43111.60833333333</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>190992588</v>
+        <v>190841520</v>
       </c>
       <c r="C14">
-        <v>21000088</v>
+        <v>20800205</v>
       </c>
       <c r="D14" s="2">
-        <v>43098.609722222223</v>
+        <v>43110.65347222222</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>191001277</v>
+        <v>190901557</v>
       </c>
       <c r="C15">
-        <v>20615095</v>
+        <v>21002510</v>
       </c>
       <c r="D15" s="2">
-        <v>43070.601388888892</v>
+        <v>43116.55972222222</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>191676884</v>
+        <v>191007290</v>
       </c>
       <c r="C16">
-        <v>20717097</v>
+        <v>21001570</v>
       </c>
       <c r="D16" s="2">
-        <v>43097.468055555553</v>
+        <v>43115.484027777777</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>191754485</v>
+        <v>191007290</v>
       </c>
       <c r="C17">
-        <v>21003597</v>
+        <v>21001580</v>
       </c>
       <c r="D17" s="2">
-        <v>43091.519444444442</v>
+        <v>43115.438194444447</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -753,461 +780,671 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>191770881</v>
+        <v>191007290</v>
       </c>
       <c r="C18">
-        <v>21700435</v>
+        <v>21002362</v>
       </c>
       <c r="D18" s="2">
-        <v>43084.668055555558</v>
+        <v>43115.442361111112</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>192381206</v>
+        <v>191007290</v>
       </c>
       <c r="C19">
-        <v>21400094</v>
+        <v>21003944</v>
       </c>
       <c r="D19" s="2">
-        <v>43085.020138888889</v>
+        <v>43115.474305555559</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20">
-        <v>192411783</v>
+        <v>191007290</v>
       </c>
       <c r="C20">
-        <v>21002524</v>
+        <v>21004085</v>
       </c>
       <c r="D20" s="2">
-        <v>43073.510416666664</v>
+        <v>43115.440972222219</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B21">
-        <v>192443064</v>
+        <v>191007290</v>
       </c>
       <c r="C21">
-        <v>21001044</v>
+        <v>21004179</v>
       </c>
       <c r="D21" s="2">
-        <v>43074.427777777775</v>
+        <v>43115.486805555556</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B22">
-        <v>192664634</v>
+        <v>191007290</v>
       </c>
       <c r="C22">
-        <v>21300126</v>
+        <v>21004183</v>
       </c>
       <c r="D22" s="2">
-        <v>43074.634027777778</v>
+        <v>43115.478472222225</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B23">
-        <v>490835990</v>
+        <v>191007290</v>
       </c>
       <c r="C23">
-        <v>20615713</v>
+        <v>21004230</v>
       </c>
       <c r="D23" s="2">
-        <v>43082.46875</v>
+        <v>43112.707638888889</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B24">
-        <v>491039642</v>
+        <v>191007290</v>
       </c>
       <c r="C24">
-        <v>21300840</v>
+        <v>21004401</v>
       </c>
       <c r="D24" s="2">
-        <v>43088.451388888891</v>
+        <v>43115.470138888886</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B25">
-        <v>491256344</v>
+        <v>191168053</v>
       </c>
       <c r="C25">
-        <v>21300762</v>
+        <v>20801768</v>
       </c>
       <c r="D25" s="2">
-        <v>43088.451388888891</v>
+        <v>43118.47152777778</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B26">
-        <v>491262486</v>
+        <v>191330469</v>
       </c>
       <c r="C26">
-        <v>21500545</v>
+        <v>21500513</v>
       </c>
       <c r="D26" s="2">
-        <v>43082.475694444445</v>
+        <v>43123.414583333331</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B27">
-        <v>690505792</v>
+        <v>191423765</v>
       </c>
       <c r="C27">
-        <v>21400300</v>
+        <v>21004063</v>
       </c>
       <c r="D27" s="2">
-        <v>43082.441666666666</v>
+        <v>43111.460416666669</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B28">
-        <v>690621783</v>
+        <v>191755729</v>
       </c>
       <c r="C28">
-        <v>21500235</v>
+        <v>21100343</v>
       </c>
       <c r="D28" s="2">
-        <v>43096.611805555556</v>
+        <v>43109.488194444442</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B29">
-        <v>690663663</v>
+        <v>191766410</v>
       </c>
       <c r="C29">
-        <v>21600019</v>
+        <v>20802073</v>
       </c>
       <c r="D29" s="2">
-        <v>43081.378472222219</v>
+        <v>43123.55</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B30">
-        <v>691437006</v>
+        <v>191981071</v>
       </c>
       <c r="C30">
-        <v>21003972</v>
+        <v>21000362</v>
       </c>
       <c r="D30" s="2">
-        <v>43083.418749999997</v>
+        <v>43109.59375</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B31">
-        <v>691806261</v>
+        <v>192342749</v>
       </c>
       <c r="C31">
-        <v>20614890</v>
+        <v>20301827</v>
       </c>
       <c r="D31" s="2">
-        <v>43097.50277777778</v>
+        <v>43112.603472222225</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B32">
-        <v>700398981</v>
+        <v>192445769</v>
       </c>
       <c r="C32">
-        <v>20800537</v>
+        <v>21400320</v>
       </c>
       <c r="D32" s="2">
-        <v>43076.531944444447</v>
+        <v>43105.470138888886</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B33">
-        <v>700847133</v>
+        <v>192694244</v>
       </c>
       <c r="C33">
-        <v>20800955</v>
+        <v>21500381</v>
       </c>
       <c r="D33" s="2">
-        <v>43096.476388888892</v>
+        <v>43117.570833333331</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B34">
-        <v>700847133</v>
+        <v>690511559</v>
       </c>
       <c r="C34">
-        <v>21000824</v>
+        <v>20614985</v>
       </c>
       <c r="D34" s="2">
-        <v>43096.478472222225</v>
+        <v>43122.592361111114</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B35">
-        <v>790250958</v>
+        <v>690566151</v>
       </c>
       <c r="C35">
-        <v>21003321</v>
+        <v>2100000000019</v>
       </c>
       <c r="D35" s="2">
-        <v>43074.711805555555</v>
+        <v>43115.613194444442</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B36">
-        <v>790384280</v>
+        <v>690639773</v>
       </c>
       <c r="C36">
-        <v>21002770</v>
+        <v>20800044</v>
       </c>
       <c r="D36" s="2">
-        <v>43075.645138888889</v>
+        <v>43117.685416666667</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B37">
-        <v>790384502</v>
+        <v>690692476</v>
       </c>
       <c r="C37">
-        <v>20900319</v>
+        <v>21500098</v>
       </c>
       <c r="D37" s="2">
-        <v>43098.606944444444</v>
+        <v>43108.501388888886</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B38">
-        <v>790457384</v>
+        <v>691085067</v>
       </c>
       <c r="C38">
-        <v>20801581</v>
+        <v>21300589</v>
       </c>
       <c r="D38" s="2">
-        <v>43097.501388888886</v>
+        <v>43104.470833333333</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B39">
-        <v>790512735</v>
+        <v>691763809</v>
       </c>
       <c r="C39">
-        <v>20700937</v>
+        <v>21100377</v>
       </c>
       <c r="D39" s="2">
-        <v>43081.615972222222</v>
+        <v>43116.529166666667</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B40">
-        <v>790674272</v>
+        <v>691817456</v>
       </c>
       <c r="C40">
-        <v>21004243</v>
+        <v>21600014</v>
       </c>
       <c r="D40" s="2">
-        <v>43076.530555555553</v>
+        <v>43111.60833333333</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B41">
-        <v>790679856</v>
+        <v>691937866</v>
       </c>
       <c r="C41">
-        <v>21000474</v>
+        <v>21400302</v>
       </c>
       <c r="D41" s="2">
-        <v>43088.450694444444</v>
+        <v>43112.422222222223</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B42">
-        <v>790789110</v>
+        <v>700067743</v>
       </c>
       <c r="C42">
-        <v>21300436</v>
+        <v>21000559</v>
       </c>
       <c r="D42" s="2">
-        <v>43080.603472222225</v>
+        <v>43112.48541666667</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B43">
-        <v>790789506</v>
+        <v>700264189</v>
       </c>
       <c r="C43">
-        <v>21001634</v>
+        <v>21000233</v>
       </c>
       <c r="D43" s="2">
-        <v>43088.479861111111</v>
+        <v>43112.617361111108</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B44">
-        <v>790810264</v>
+        <v>700320855</v>
       </c>
       <c r="C44">
-        <v>20801781</v>
+        <v>20614772</v>
       </c>
       <c r="D44" s="2">
-        <v>43095.423611111109</v>
+        <v>43111.649305555555</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B45">
-        <v>790852448</v>
+        <v>700847120</v>
       </c>
       <c r="C45">
-        <v>21004184</v>
+        <v>20802045</v>
       </c>
       <c r="D45" s="2">
-        <v>43073.495138888888</v>
+        <v>43116.462500000001</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B46">
-        <v>790911901</v>
+        <v>790006703</v>
       </c>
       <c r="C46">
-        <v>21300078</v>
+        <v>21400164</v>
       </c>
       <c r="D46" s="2">
-        <v>43081.350694444445</v>
+        <v>43119.459722222222</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B47">
-        <v>790991020</v>
+        <v>790192462</v>
       </c>
       <c r="C47">
-        <v>20717215</v>
+        <v>20801595</v>
       </c>
       <c r="D47" s="2">
-        <v>43077.649305555555</v>
+        <v>43112.486111111109</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B48">
-        <v>791000901</v>
+        <v>790257383</v>
       </c>
       <c r="C48">
-        <v>21400137</v>
+        <v>21003911</v>
       </c>
       <c r="D48" s="2">
-        <v>43090.425000000003</v>
+        <v>43123.515972222223</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B49">
-        <v>791037437</v>
+        <v>790280302</v>
       </c>
       <c r="C49">
-        <v>21001753</v>
+        <v>21000213</v>
       </c>
       <c r="D49" s="2">
-        <v>43070.617361111108</v>
+        <v>43115.613888888889</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50">
+        <v>790314844</v>
+      </c>
+      <c r="C50">
+        <v>21002312</v>
+      </c>
+      <c r="D50" s="2">
+        <v>43120.544444444444</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51">
+        <v>790321053</v>
+      </c>
+      <c r="C51">
+        <v>21300147</v>
+      </c>
+      <c r="D51" s="2">
+        <v>43122.583333333336</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52">
+        <v>790330140</v>
+      </c>
+      <c r="C52">
+        <v>21200189</v>
+      </c>
+      <c r="D52" s="2">
+        <v>43115.40625</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53">
+        <v>790384081</v>
+      </c>
+      <c r="C53">
+        <v>21003539</v>
+      </c>
+      <c r="D53" s="2">
+        <v>43120.356249999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54">
+        <v>790396683</v>
+      </c>
+      <c r="C54">
+        <v>21001355</v>
+      </c>
+      <c r="D54" s="2">
+        <v>43119.484722222223</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>48</v>
       </c>
-      <c r="B50">
-        <v>791037970</v>
-      </c>
-      <c r="C50">
-        <v>21400443</v>
-      </c>
-      <c r="D50" s="2">
-        <v>43097.506249999999</v>
+      <c r="B55">
+        <v>790398446</v>
+      </c>
+      <c r="C55">
+        <v>20701017</v>
+      </c>
+      <c r="D55" s="2">
+        <v>43103.475694444445</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56">
+        <v>790489433</v>
+      </c>
+      <c r="C56">
+        <v>20800409</v>
+      </c>
+      <c r="D56" s="2">
+        <v>43116.637499999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>50</v>
+      </c>
+      <c r="B57">
+        <v>790610462</v>
+      </c>
+      <c r="C57">
+        <v>21400257</v>
+      </c>
+      <c r="D57" s="2">
+        <v>43116.564583333333</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>51</v>
+      </c>
+      <c r="B58">
+        <v>790851758</v>
+      </c>
+      <c r="C58">
+        <v>21001665</v>
+      </c>
+      <c r="D58" s="2">
+        <v>43110.606249999997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59">
+        <v>790900028</v>
+      </c>
+      <c r="C59">
+        <v>21300228</v>
+      </c>
+      <c r="D59" s="2">
+        <v>43119.630555555559</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>53</v>
+      </c>
+      <c r="B60">
+        <v>790914209</v>
+      </c>
+      <c r="C60">
+        <v>21300073</v>
+      </c>
+      <c r="D60" s="2">
+        <v>43105.556944444441</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61">
+        <v>790914209</v>
+      </c>
+      <c r="C61">
+        <v>21400148</v>
+      </c>
+      <c r="D61" s="2">
+        <v>43105.557638888888</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>54</v>
+      </c>
+      <c r="B62">
+        <v>790968576</v>
+      </c>
+      <c r="C62">
+        <v>21500598</v>
+      </c>
+      <c r="D62" s="2">
+        <v>43118.647916666669</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>55</v>
+      </c>
+      <c r="B63">
+        <v>790969159</v>
+      </c>
+      <c r="C63">
+        <v>21400196</v>
+      </c>
+      <c r="D63" s="2">
+        <v>43108.474305555559</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>56</v>
+      </c>
+      <c r="B64">
+        <v>791014725</v>
+      </c>
+      <c r="C64">
+        <v>21003555</v>
+      </c>
+      <c r="D64" s="2">
+        <v>43117.593055555553</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>57</v>
+      </c>
+      <c r="B65">
+        <v>791038780</v>
+      </c>
+      <c r="C65">
+        <v>2100000000095</v>
+      </c>
+      <c r="D65" s="2">
+        <v>43112.484722222223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>